<commit_message>
Set pending invoice item interval
</commit_message>
<xml_diff>
--- a/server/functions/test/HourlySchedule.xlsx
+++ b/server/functions/test/HourlySchedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rz/Documents/code/gmind/clubsports/TourneyMaster/server/functions/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AB2D2F-1EB8-D94B-82E7-6785BADFE24D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC18BC9B-FF14-5049-BBD2-AEB32600CF80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{BD051CE2-A9ED-B449-8B72-E257B35AED4C}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16220" xr2:uid="{BD051CE2-A9ED-B449-8B72-E257B35AED4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01A41FF-50D7-FF4B-97C4-DFC4814FCCD9}">
-  <dimension ref="B3:B8"/>
+  <dimension ref="A3:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -382,39 +382,54 @@
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3">
-        <v>1592504000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+        <v>1592656000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4">
         <f>B3+3600</f>
-        <v>1592507600</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+        <v>1592659600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5">
         <f t="shared" ref="B5:B8" si="0">B4+3600</f>
-        <v>1592511200</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+        <v>1592663200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="B6">
         <f>B5+3600</f>
-        <v>1592514800</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+        <v>1592666800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>1592518400</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+        <v>1592670400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>1592522000</v>
+        <v>1592674000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>